<commit_message>
data update july 22
</commit_message>
<xml_diff>
--- a/Immigration Filings/COVID-19_Related_Immigration_Filings.xlsx
+++ b/Immigration Filings/COVID-19_Related_Immigration_Filings.xlsx
@@ -8021,13 +8021,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBD4567B-DF40-438B-8DB9-8B4D4AB91087}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96A68091-ED86-42D8-860C-1DA420B57A34}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82DCC6DC-1C43-4AC5-83B0-F708C6ABB42C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5CEA086-2A7A-403B-B113-C10BF6A22EBC}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A17BAA62-3200-4CF4-BEF8-387564496AD5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B261A05D-0596-4CF7-86BB-C015F67B6936}"/>
 </file>
</xml_diff>